<commit_message>
Update 3NF Excel file with new data
</commit_message>
<xml_diff>
--- a/3NF.xlsx
+++ b/3NF.xlsx
@@ -5,18 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KedirBiruh\Desktop\Normalisierung\normalisierung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KedirBiruh\Desktop\Datenbank\normalisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A40233F-9FBF-4DC0-90CD-2C7183A00E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B78FE4-6427-491A-B562-E6A6270B70C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{4E33EA83-0576-4B84-9E67-A012B75C64C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{4E33EA83-0576-4B84-9E67-A012B75C64C1}"/>
   </bookViews>
   <sheets>
     <sheet name="UF" sheetId="3" r:id="rId1"/>
     <sheet name="1NF" sheetId="2" r:id="rId2"/>
     <sheet name="2NF" sheetId="4" r:id="rId3"/>
     <sheet name="3NF" sheetId="5" r:id="rId4"/>
+    <sheet name="Kunden" sheetId="6" r:id="rId5"/>
+    <sheet name="Produkte" sheetId="7" r:id="rId6"/>
+    <sheet name="Bestellungen" sheetId="8" r:id="rId7"/>
+    <sheet name="Bestellpositionen" sheetId="9" r:id="rId8"/>
+    <sheet name="Städte" sheetId="10" r:id="rId9"/>
+    <sheet name="Hersteller" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="183">
   <si>
     <t>Unnormalisierte Bestelldaten</t>
   </si>
@@ -525,12 +531,6 @@
     <t>Kundennummer(FK)</t>
   </si>
   <si>
-    <t>Bestellnummer(PK/FK)</t>
-  </si>
-  <si>
-    <t>Produktnummer(pk7FK)</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
@@ -592,12 +592,18 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Produktnummer(PK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -714,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -770,15 +776,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2283,6 +2291,134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3675A8D3-E810-40F7-BD30-85F39F4860D0}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FC7524-13A1-488E-BD9D-C841DB370BD7}">
   <dimension ref="A1:P43"/>
@@ -2331,10 +2467,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -2381,10 +2517,10 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F4" t="s">
         <v>119</v>
@@ -2491,10 +2627,10 @@
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F6" t="s">
         <v>122</v>
@@ -2601,10 +2737,10 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F8" t="s">
         <v>119</v>
@@ -2651,10 +2787,10 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
         <v>124</v>
@@ -2761,10 +2897,10 @@
         <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
         <v>127</v>
@@ -2811,10 +2947,10 @@
         <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F12" t="s">
         <v>122</v>
@@ -2861,10 +2997,10 @@
         <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F13" t="s">
         <v>130</v>
@@ -3031,10 +3167,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F16" t="s">
         <v>119</v>
@@ -3081,10 +3217,10 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F17" t="s">
         <v>124</v>
@@ -3131,10 +3267,10 @@
         <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F18" t="s">
         <v>132</v>
@@ -3241,10 +3377,10 @@
         <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F20" t="s">
         <v>134</v>
@@ -3291,10 +3427,10 @@
         <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F21" t="s">
         <v>130</v>
@@ -3341,10 +3477,10 @@
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F22" t="s">
         <v>122</v>
@@ -3391,10 +3527,10 @@
         <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F23" t="s">
         <v>136</v>
@@ -3501,10 +3637,10 @@
         <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F25" t="s">
         <v>136</v>
@@ -3551,10 +3687,10 @@
         <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F26" t="s">
         <v>138</v>
@@ -3661,10 +3797,10 @@
         <v>111</v>
       </c>
       <c r="D28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F28" t="s">
         <v>140</v>
@@ -3711,10 +3847,10 @@
         <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F29" t="s">
         <v>119</v>
@@ -3821,10 +3957,10 @@
         <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F31" t="s">
         <v>132</v>
@@ -3871,10 +4007,10 @@
         <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F32" t="s">
         <v>136</v>
@@ -4123,10 +4259,10 @@
         <v>147</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -4179,10 +4315,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>119</v>
@@ -4235,10 +4371,10 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>122</v>
@@ -4292,10 +4428,10 @@
         <v>38</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>124</v>
@@ -4348,10 +4484,10 @@
         <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>127</v>
@@ -4405,10 +4541,10 @@
         <v>59</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>130</v>
@@ -4461,10 +4597,10 @@
         <v>73</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>132</v>
@@ -4517,10 +4653,10 @@
         <v>85</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>134</v>
@@ -4574,10 +4710,10 @@
         <v>94</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>136</v>
@@ -4630,10 +4766,10 @@
         <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>138</v>
@@ -4686,10 +4822,10 @@
         <v>111</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>140</v>
@@ -5135,8 +5271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F368A742-77EE-48A7-AC70-2F4FE20B1598}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5179,10 +5315,10 @@
         <v>147</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -5215,10 +5351,10 @@
         <v>12</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="S2" s="14" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="T2" s="14" t="s">
         <v>8</v>
@@ -5229,10 +5365,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>119</v>
@@ -5279,10 +5415,10 @@
         <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>122</v>
@@ -5330,10 +5466,10 @@
         <v>38</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>124</v>
@@ -5380,10 +5516,10 @@
         <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>127</v>
@@ -5431,10 +5567,10 @@
         <v>59</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>130</v>
@@ -5481,10 +5617,10 @@
         <v>73</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>132</v>
@@ -5531,10 +5667,10 @@
         <v>85</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>134</v>
@@ -5582,10 +5718,10 @@
         <v>94</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>136</v>
@@ -5632,10 +5768,10 @@
         <v>100</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>138</v>
@@ -5682,10 +5818,10 @@
         <v>111</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>140</v>
@@ -6054,7 +6190,6 @@
       <c r="B28" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="C28" s="25"/>
       <c r="G28" s="3" t="s">
         <v>151</v>
       </c>
@@ -6078,7 +6213,6 @@
       <c r="B29" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C29" s="26"/>
       <c r="G29" s="4" t="s">
         <v>20</v>
       </c>
@@ -6104,7 +6238,6 @@
       <c r="B30" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="26"/>
       <c r="G30" s="5" t="s">
         <v>26</v>
       </c>
@@ -6128,7 +6261,6 @@
       <c r="B31" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="27"/>
       <c r="G31" s="5" t="s">
         <v>35</v>
       </c>
@@ -6152,7 +6284,6 @@
       <c r="B32" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C32" s="27"/>
       <c r="G32" s="5" t="s">
         <v>44</v>
       </c>
@@ -6177,7 +6308,6 @@
       <c r="B33" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="27"/>
       <c r="G33" s="4" t="s">
         <v>44</v>
       </c>
@@ -6202,7 +6332,6 @@
       <c r="B34" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="26"/>
       <c r="G34" s="5" t="s">
         <v>56</v>
       </c>
@@ -6219,7 +6348,6 @@
       <c r="B35" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C35" s="26"/>
       <c r="G35" s="5" t="s">
         <v>65</v>
       </c>
@@ -6234,7 +6362,6 @@
       <c r="B36" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="27"/>
       <c r="G36" s="4" t="s">
         <v>65</v>
       </c>
@@ -6249,7 +6376,6 @@
       <c r="B37" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="26"/>
       <c r="G37" s="4" t="s">
         <v>26</v>
       </c>
@@ -6312,6 +6438,1242 @@
     <row r="55" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q55" s="10"/>
       <c r="S55"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38D32C2-59E2-4EB9-ACDF-CAB52EC707DA}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D928848-B565-4070-87B3-EE32214ECB2D}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1200</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5">
+        <v>25.5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2500</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="4">
+        <v>150</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5">
+        <v>350</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="5">
+        <v>180</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="4">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="4">
+        <v>60</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="5">
+        <v>95</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="4">
+        <v>750</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="5">
+        <v>159.99</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B62B76E-6D7F-48A9-8D9C-1E8C1B1066CB}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="29" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1001</v>
+      </c>
+      <c r="B3" s="27">
+        <v>45672</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>1002</v>
+      </c>
+      <c r="B4" s="27">
+        <v>45673</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>1003</v>
+      </c>
+      <c r="B5" s="27">
+        <v>45674</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>1004</v>
+      </c>
+      <c r="B6" s="28">
+        <v>45675</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>1005</v>
+      </c>
+      <c r="B7" s="28">
+        <v>45676</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="18">
+        <v>1006</v>
+      </c>
+      <c r="B8" s="27">
+        <v>45677</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>1007</v>
+      </c>
+      <c r="B9" s="28">
+        <v>45678</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="5">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
+        <v>1008</v>
+      </c>
+      <c r="B10" s="27">
+        <v>45689</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>1009</v>
+      </c>
+      <c r="B11" s="28">
+        <v>45690</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="18">
+        <v>1010</v>
+      </c>
+      <c r="B12" s="27">
+        <v>45691</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <v>1011</v>
+      </c>
+      <c r="B13" s="27">
+        <v>45692</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="4">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <v>1012</v>
+      </c>
+      <c r="B14" s="28">
+        <v>45693</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>1013</v>
+      </c>
+      <c r="B15" s="27">
+        <v>45694</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>1014</v>
+      </c>
+      <c r="B16" s="28">
+        <v>45695</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>1015</v>
+      </c>
+      <c r="B17" s="28">
+        <v>45696</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18">
+        <v>1016</v>
+      </c>
+      <c r="B18" s="27">
+        <v>45697</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="4">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <v>1017</v>
+      </c>
+      <c r="B19" s="27">
+        <v>45698</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="4">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>1018</v>
+      </c>
+      <c r="B20" s="28">
+        <v>45699</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>1019</v>
+      </c>
+      <c r="B21" s="28">
+        <v>45700</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="5">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="18">
+        <v>1020</v>
+      </c>
+      <c r="B22" s="27">
+        <v>45701</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B21F5A2-6B43-4255-A07B-FF7E1C93F228}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1001</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <f>A3</f>
+        <v>1001</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>1002</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <f>A5</f>
+        <v>1002</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>1003</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>1004</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <f>A8</f>
+        <v>1004</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <v>1005</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="18">
+        <v>1006</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>1007</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="18">
+        <f t="shared" ref="A13:A14" si="0">A12</f>
+        <v>1007</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <f t="shared" si="0"/>
+        <v>1007</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="18">
+        <v>1008</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>1009</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>1010</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <f>A17</f>
+        <v>1010</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="18">
+        <v>1011</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>1012</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="18">
+        <v>1013</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
+        <v>1014</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="18">
+        <f>A22</f>
+        <v>1014</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
+        <v>1015</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="18">
+        <v>1016</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <f>A25</f>
+        <v>1016</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="18">
+        <v>1017</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
+        <v>1018</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="18">
+        <f>A28</f>
+        <v>1018</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="20">
+        <v>1019</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="18">
+        <v>1020</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
+        <f t="shared" ref="A32:A33" si="1">A31</f>
+        <v>1020</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="18">
+        <f t="shared" si="1"/>
+        <v>1020</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E81DA7-3B89-48A5-977A-9CF9C09F85D9}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>121</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update 3NF Excel file and add temporary file for editing
</commit_message>
<xml_diff>
--- a/3NF.xlsx
+++ b/3NF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KedirBiruh\Desktop\Datenbank\normalisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B78FE4-6427-491A-B562-E6A6270B70C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B22E8D-6B19-4FBA-B2D7-7A52FADEEC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{4E33EA83-0576-4B84-9E67-A012B75C64C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="9" xr2:uid="{4E33EA83-0576-4B84-9E67-A012B75C64C1}"/>
   </bookViews>
   <sheets>
     <sheet name="UF" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="183">
   <si>
     <t>Unnormalisierte Bestelldaten</t>
   </si>
@@ -602,7 +602,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -720,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -776,17 +776,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2293,10 +2289,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3675A8D3-E810-40F7-BD30-85F39F4860D0}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,112 +2301,99 @@
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>153</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
+      <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>36</v>
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>45</v>
+      <c r="A7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
+      <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
+      <c r="A10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6447,9 +6430,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D38D32C2-59E2-4EB9-ACDF-CAB52EC707DA}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6460,199 +6445,190 @@
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>155</v>
+      <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>162</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>123</v>
+      <c r="A4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>131</v>
+      <c r="A7" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>135</v>
+      <c r="A9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>137</v>
+      <c r="A10" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E12" s="4" t="s">
         <v>128</v>
       </c>
     </row>
@@ -6663,10 +6639,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D928848-B565-4070-87B3-EE32214ECB2D}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6677,193 +6653,171 @@
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4">
+        <v>1200</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>149</v>
+      <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5">
+        <v>25.5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4">
-        <v>1200</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
+      <c r="A3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C4" s="5">
-        <v>25.5</v>
+        <v>2500</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="5">
-        <v>45</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>35</v>
+      <c r="A5" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="4">
+        <v>150</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C6" s="5">
-        <v>2500</v>
+        <v>350</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="4">
-        <v>150</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>44</v>
+      <c r="A7" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="5">
+        <v>180</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="5">
-        <v>350</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>56</v>
+      <c r="A8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="4">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="5">
-        <v>180</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>65</v>
+      <c r="A9" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="4">
+        <v>60</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="4">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>65</v>
+      <c r="A10" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="5">
+        <v>95</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C11" s="4">
-        <v>60</v>
+        <v>750</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C12" s="5">
-        <v>95</v>
+        <v>159.99</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="4">
-        <v>750</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C14" s="5">
-        <v>159.99</v>
-      </c>
-      <c r="D14" s="5" t="s">
         <v>110</v>
       </c>
     </row>
@@ -6874,309 +6828,297 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B62B76E-6D7F-48A9-8D9C-1E8C1B1066CB}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="27" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18">
+        <v>1001</v>
+      </c>
+      <c r="B1" s="25">
+        <v>45672</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4">
+        <v>5.99</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="18">
+        <v>1002</v>
+      </c>
+      <c r="B2" s="25">
+        <v>45673</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4">
+        <v>5.99</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
-        <v>1001</v>
-      </c>
-      <c r="B3" s="27">
-        <v>45672</v>
+        <v>1003</v>
+      </c>
+      <c r="B3" s="25">
+        <v>45674</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="4">
-        <v>5.99</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
-        <v>1002</v>
-      </c>
-      <c r="B4" s="27">
-        <v>45673</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="20">
+        <v>1004</v>
+      </c>
+      <c r="B4" s="26">
+        <v>45675</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>1005</v>
+      </c>
+      <c r="B5" s="26">
+        <v>45676</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>1006</v>
+      </c>
+      <c r="B6" s="25">
+        <v>45677</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="4">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
-        <v>1003</v>
-      </c>
-      <c r="B5" s="27">
-        <v>45674</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>4.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
-        <v>1004</v>
-      </c>
-      <c r="B6" s="28">
-        <v>45675</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="5">
-        <v>12.99</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
-        <v>1005</v>
-      </c>
-      <c r="B7" s="28">
-        <v>45676</v>
+        <v>1007</v>
+      </c>
+      <c r="B7" s="26">
+        <v>45678</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D7" s="5">
-        <v>9.99</v>
+        <v>7.99</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
-        <v>1006</v>
-      </c>
-      <c r="B8" s="27">
-        <v>45677</v>
+        <v>1008</v>
+      </c>
+      <c r="B8" s="25">
+        <v>45689</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4">
-        <v>4.99</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
-        <v>1007</v>
-      </c>
-      <c r="B9" s="28">
-        <v>45678</v>
+        <v>1009</v>
+      </c>
+      <c r="B9" s="26">
+        <v>45690</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5">
-        <v>7.99</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
-        <v>1008</v>
-      </c>
-      <c r="B10" s="27">
-        <v>45689</v>
+        <v>1010</v>
+      </c>
+      <c r="B10" s="25">
+        <v>45691</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D10" s="4">
-        <v>9.99</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
-        <v>1009</v>
-      </c>
-      <c r="B11" s="28">
-        <v>45690</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="5">
-        <v>9.99</v>
+      <c r="A11" s="18">
+        <v>1011</v>
+      </c>
+      <c r="B11" s="25">
+        <v>45692</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="4">
+        <v>15.99</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
-        <v>1010</v>
-      </c>
-      <c r="B12" s="27">
-        <v>45691</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="4">
-        <v>4.99</v>
+      <c r="A12" s="20">
+        <v>1012</v>
+      </c>
+      <c r="B12" s="26">
+        <v>45693</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5.99</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
-        <v>1011</v>
-      </c>
-      <c r="B13" s="27">
-        <v>45692</v>
+        <v>1013</v>
+      </c>
+      <c r="B13" s="25">
+        <v>45694</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="D13" s="4">
-        <v>15.99</v>
+        <v>4.99</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
-        <v>1012</v>
-      </c>
-      <c r="B14" s="28">
-        <v>45693</v>
+        <v>1014</v>
+      </c>
+      <c r="B14" s="26">
+        <v>45695</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="D14" s="5">
         <v>5.99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
-        <v>1013</v>
-      </c>
-      <c r="B15" s="27">
-        <v>45694</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4">
-        <v>4.99</v>
+      <c r="A15" s="20">
+        <v>1015</v>
+      </c>
+      <c r="B15" s="26">
+        <v>45696</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="5">
+        <v>5.99</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
-        <v>1014</v>
-      </c>
-      <c r="B16" s="28">
-        <v>45695</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="A16" s="18">
+        <v>1016</v>
+      </c>
+      <c r="B16" s="25">
+        <v>45697</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="4">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>1017</v>
+      </c>
+      <c r="B17" s="25">
+        <v>45698</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="4">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>1018</v>
+      </c>
+      <c r="B18" s="26">
+        <v>45699</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="5">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>1019</v>
+      </c>
+      <c r="B19" s="26">
+        <v>45700</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="5">
+        <v>5.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18">
+        <v>1020</v>
+      </c>
+      <c r="B20" s="25">
+        <v>45701</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="5">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
-        <v>1015</v>
-      </c>
-      <c r="B17" s="28">
-        <v>45696</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="5">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
-        <v>1016</v>
-      </c>
-      <c r="B18" s="27">
-        <v>45697</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="4">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>1017</v>
-      </c>
-      <c r="B19" s="27">
-        <v>45698</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D19" s="4">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
-        <v>1018</v>
-      </c>
-      <c r="B20" s="28">
-        <v>45699</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="5">
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
-        <v>1019</v>
-      </c>
-      <c r="B21" s="28">
-        <v>45700</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="5">
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
-        <v>1020</v>
-      </c>
-      <c r="B22" s="27">
-        <v>45701</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="D20" s="4">
         <v>5.99</v>
       </c>
     </row>
@@ -7188,10 +7130,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B21F5A2-6B43-4255-A07B-FF7E1C93F228}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="L20" sqref="L20:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7201,27 +7143,32 @@
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="7"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="18">
+        <v>1001</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>8</v>
+      <c r="A2" s="20">
+        <f>A1</f>
+        <v>1001</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>17</v>
@@ -7233,21 +7180,21 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <f>A3</f>
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C4" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C5" s="15">
         <v>1</v>
@@ -7255,22 +7202,22 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
-        <f>A5</f>
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C6" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
-        <v>1003</v>
+        <f>A6</f>
+        <v>1004</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C7" s="15">
         <v>1</v>
@@ -7278,22 +7225,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C8" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
-        <f>A8</f>
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C9" s="15">
         <v>1</v>
@@ -7301,32 +7247,34 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C10" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
-        <v>1006</v>
+        <f t="shared" ref="A11:A12" si="0">A10</f>
+        <v>1007</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C11" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
+        <f t="shared" si="0"/>
         <v>1007</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="C12" s="16">
         <v>1</v>
@@ -7334,23 +7282,21 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
-        <f t="shared" ref="A13:A14" si="0">A12</f>
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C13" s="15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
-        <f t="shared" si="0"/>
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C14" s="16">
         <v>1</v>
@@ -7358,10 +7304,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="C15" s="15">
         <v>1</v>
@@ -7369,10 +7315,11 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
-        <v>1009</v>
+        <f>A15</f>
+        <v>1010</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="C16" s="16">
         <v>1</v>
@@ -7380,10 +7327,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="C17" s="15">
         <v>1</v>
@@ -7391,11 +7338,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
-        <f>A17</f>
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>
@@ -7403,10 +7349,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
@@ -7414,21 +7360,22 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C20" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
-        <v>1013</v>
+        <f>A20</f>
+        <v>1014</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C21" s="15">
         <v>1</v>
@@ -7436,22 +7383,21 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C22" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
-        <f>A22</f>
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="C23" s="15">
         <v>1</v>
@@ -7459,10 +7405,11 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
-        <v>1015</v>
+        <f>A23</f>
+        <v>1016</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="C24" s="16">
         <v>1</v>
@@ -7470,10 +7417,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="C25" s="15">
         <v>1</v>
@@ -7481,11 +7428,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
-        <f>A25</f>
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="C26" s="16">
         <v>1</v>
@@ -7493,10 +7439,11 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
-        <v>1017</v>
+        <f>A26</f>
+        <v>1018</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="C27" s="15">
         <v>1</v>
@@ -7504,10 +7451,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C28" s="16">
         <v>1</v>
@@ -7515,11 +7462,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
-        <f>A28</f>
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="C29" s="15">
         <v>1</v>
@@ -7527,10 +7473,11 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
-        <v>1019</v>
+        <f t="shared" ref="A30:A31" si="1">A29</f>
+        <v>1020</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C30" s="16">
         <v>1</v>
@@ -7538,36 +7485,13 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
-        <v>1020</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="20">
-        <f t="shared" ref="A32:A33" si="1">A31</f>
-        <v>1020</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="18">
         <f t="shared" si="1"/>
         <v>1020</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C31" s="15">
         <v>1</v>
       </c>
     </row>
@@ -7578,10 +7502,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E81DA7-3B89-48A5-977A-9CF9C09F85D9}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7591,87 +7515,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>158</v>
+      <c r="A1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>156</v>
+      <c r="A2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>121</v>
+      <c r="A3" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>121</v>
+      <c r="A4" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="15" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove old online shop SQL file and temporary Excel files; update 3NF Excel file.
</commit_message>
<xml_diff>
--- a/3NF.xlsx
+++ b/3NF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KedirBiruh\Desktop\Datenbank\normalisierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B22E8D-6B19-4FBA-B2D7-7A52FADEEC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1521440-625B-427A-A711-6BBFF1DFB1C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="9" xr2:uid="{4E33EA83-0576-4B84-9E67-A012B75C64C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{4E33EA83-0576-4B84-9E67-A012B75C64C1}"/>
   </bookViews>
   <sheets>
     <sheet name="UF" sheetId="3" r:id="rId1"/>
@@ -2291,7 +2291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3675A8D3-E810-40F7-BD30-85F39F4860D0}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
@@ -5254,8 +5254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F368A742-77EE-48A7-AC70-2F4FE20B1598}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27:H40"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N31" sqref="N30:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6150,7 +6150,7 @@
       </c>
     </row>
     <row r="27" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="7" t="s">
         <v>158</v>
       </c>
       <c r="G27" s="7" t="s">

</xml_diff>